<commit_message>
Added Rule based data
</commit_message>
<xml_diff>
--- a/Test Data Per Error Type.xlsx
+++ b/Test Data Per Error Type.xlsx
@@ -10,15 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="662">
   <si>
     <t>Insertion</t>
   </si>
@@ -1902,9 +1901,6 @@
     <t>Lemmas</t>
   </si>
   <si>
-    <t>For Chef 1</t>
-  </si>
-  <si>
     <t>Chicoy 2</t>
   </si>
   <si>
@@ -1927,13 +1923,136 @@
   </si>
   <si>
     <t>Kung kung masaktan</t>
+  </si>
+  <si>
+    <t>Mga balita tungkol sa laki ng Birgus latro at higit sa lahat, umabot ng 4kg ang bigat nito, humaba ng 400mm ang katawan, at 2m ang haba ng binti nito sa lahat ng lalaking tatos na masmalaki pa sa babaeng tatos.</t>
+  </si>
+  <si>
+    <t>masmalaki</t>
+  </si>
+  <si>
+    <t>mas malaki</t>
+  </si>
+  <si>
+    <t>Chef 1</t>
+  </si>
+  <si>
+    <t>Tulad ng mga uwang, malalaki at malalakas ang kasunod ng pares na binti nito na pwede silang umakyat ng patayo sa mga puno hanggang anim na metro pataas (palaging nasa puno ng niyog)</t>
+  </si>
+  <si>
+    <t>umakyat ng patayo</t>
+  </si>
+  <si>
+    <t>umakyat nang patayo</t>
+  </si>
+  <si>
+    <t>Ibanez, Mark Denzel</t>
+  </si>
+  <si>
+    <t>Gayunman, kakain sila ng mahigit kahit anung organic, kasama ang mga dahon, gapok na prutas, itlog ng pagong, patay na hayop, at kartutso ng ibang hayop, na napaniwalaang nagbibigay ng calcium</t>
+  </si>
+  <si>
+    <t>anung</t>
+  </si>
+  <si>
+    <t>anong</t>
+  </si>
+  <si>
+    <t>Pagkatapos, iikutin niya at gagamitin ang masmaliit na sipit sa kanyang kabilang binti para hilain palabas ang putting laman ng niyog.</t>
+  </si>
+  <si>
+    <t>masmaliit</t>
+  </si>
+  <si>
+    <t>mas maliit</t>
+  </si>
+  <si>
+    <t>Lalabas rin ang tatus ng maarawn kapag mahalumigmig ang panahon o umuulan, mula pa pwede na ang kondisyon nilang huminga ng masmadali</t>
+  </si>
+  <si>
+    <t>masmadali</t>
+  </si>
+  <si>
+    <t>mas madali</t>
+  </si>
+  <si>
+    <t>Pinakamalaki at pinakamabuting na pananatili ng populasyon sa buong mundo ang Christmas Island sa karagatan ng India.</t>
+  </si>
+  <si>
+    <t>na pananatili</t>
+  </si>
+  <si>
+    <t>napananatili</t>
+  </si>
+  <si>
+    <t>Ang pag aaral sa sekswalidad ng mga hayop (lalo na ang sekswalidad sa mga primado) ay umuunlad na nang mabilis.</t>
+  </si>
+  <si>
+    <t>pag aaral</t>
+  </si>
+  <si>
+    <t>Ivan Marlowe L. Demabildo</t>
+  </si>
+  <si>
+    <t>Kahit binatikos siya, ang ideya niya ang nagpapakita ng kahirapan at imperpeksyon sa kasalukuyang tugon sa mga pagkaka-iba nito.</t>
+  </si>
+  <si>
+    <t>pagkaka-iba</t>
+  </si>
+  <si>
+    <t>pagkakaiba</t>
+  </si>
+  <si>
+    <t>Negosyong Interes-kita(pag-kuha ng deposito mula sa pagtitingi ng mga mamimili para sa pautang para sa korporeyts) ang pangunahing pagkakakilala dito bagaman unti-unti itong nagiging lugar na hindi-interes-kita tulad ng personal na pautang, pamamahala sa kayamanan at iba pang serbisyong pinansyal sa kasalukuyang mga taon.</t>
+  </si>
+  <si>
+    <t>pag-kuha</t>
+  </si>
+  <si>
+    <t>pagkuha</t>
+  </si>
+  <si>
+    <t>Christopher Edmund V. Wong</t>
+  </si>
+  <si>
+    <t>Natuklasan ito noong 1968 at Ilinarawan noong 1972. Isa ito sa pinaka bagong uri ng New World Warbler (Parulidae Family) na nailarawan.</t>
+  </si>
+  <si>
+    <t>pinaka bagong</t>
+  </si>
+  <si>
+    <t>pinakabagong</t>
+  </si>
+  <si>
+    <t>Maria Illurosa R. Lim</t>
+  </si>
+  <si>
+    <t>Pinagmasdan niya ang pagka-ayon ng limang dahon ng bulaklak at kung paano lumikha ng labis na damdamin ang pagkakatulad nito.</t>
+  </si>
+  <si>
+    <t>pagka-ayon</t>
+  </si>
+  <si>
+    <t>pagkaayon</t>
+  </si>
+  <si>
+    <t>Tsoi, Jeanine Beatrice L.</t>
+  </si>
+  <si>
+    <t>Kapag ipinapakita naman ang watawat sa labas ng isang gusali, ginagamit na puntong pangtukoy ng kaliwan at kanang bahagi ng watawat ang kaliwa at kanang tagiliran ng isang tao, kung saan nakaharap siya sa harap ng pasukan ng gusali.</t>
+  </si>
+  <si>
+    <t>pangtukoy</t>
+  </si>
+  <si>
+    <t>pantukoy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1944,6 +2063,13 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2037,7 +2163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2129,6 +2255,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7706,10 +7838,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7721,9 +7853,10 @@
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="42" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -7746,9 +7879,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>169</v>
@@ -7764,18 +7897,18 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="5" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>617</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>618</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>34</v>
@@ -7785,12 +7918,12 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>172</v>
@@ -7806,15 +7939,15 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
+        <v>619</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>620</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>621</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>182</v>
@@ -7827,118 +7960,298 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+        <v>613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>621</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>622</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>623</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>625</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>626</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>627</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>629</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>630</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>631</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>632</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>633</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>634</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>635</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>636</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>637</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>638</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>639</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>640</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>641</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>642</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>644</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>645</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>646</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>648</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>649</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>651</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>652</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>653</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>655</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>656</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>657</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>659</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>660</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>661</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="F17" s="6"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -7947,7 +8260,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -7956,7 +8269,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -7965,7 +8278,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -7974,7 +8287,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -7983,7 +8296,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -7992,7 +8305,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -8001,7 +8314,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -8010,7 +8323,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -8019,7 +8332,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -8028,7 +8341,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -8037,7 +8350,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -8046,7 +8359,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -8055,7 +8368,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -8064,7 +8377,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -8211,29 +8524,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>614</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>